<commit_message>
using the google finance to scrape
</commit_message>
<xml_diff>
--- a/stockwebscrapper/stock_prices.xlsx
+++ b/stockwebscrapper/stock_prices.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,207 +451,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>CHR.TO</t>
+          <t>CHR:TSE</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>3.1900</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>HUT.TO</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>26.39</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>GWO.TO</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>47.55</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>CGX.TO</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>10.39</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>BB.TO</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>3.2100</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>VRN.TO</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>7.47</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>TLRY.TO</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>2.1500</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>PXT.TO</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>14.28</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>AC.TO</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>23.66</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>SU.TO</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>54.75</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>BEN</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>20.16</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>ACB.TO</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>7.14</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>OGI.TO</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>2.2650</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>POU.TO</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>26.27</t>
+          <t>$3.35</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
changed  stock source to google finance
</commit_message>
<xml_diff>
--- a/stockwebscrapper/stock_prices.xlsx
+++ b/stockwebscrapper/stock_prices.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,7 +456,292 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>$3.35</t>
+          <t>$3.01</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>HUT:TSE</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>$30.85</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>GWO:TSE</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>$47.50</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>CGX:TSE</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>$12.16</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>BB:TSE</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>$5.51</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>VRN:TSE</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>$7.17</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>TLRY:TSE</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>$1.96</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>PXT:TSE</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>$13.67</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>AC:TSE</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>$22.25</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>SU:TSE</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>$50.71</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>BEN:NYSE</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>$20.11</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>ACB:TSE</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>$6.03</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>OGI:TSE</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>$2.27</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>POU:TSE</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>$31.22</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>ASM:TSE</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>$1.25</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>QCLN:NASDAQ</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>$34.47</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>AMAT:NASDAQ</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>$163.64</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>OGI:TSE</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>$2.27</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>POU:TSE</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>$31.22</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>QQC:TSE</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>$36.15</t>
         </is>
       </c>
     </row>

</xml_diff>